<commit_message>
Add Reference information based on assignment instruction to the CorrGrid file
</commit_message>
<xml_diff>
--- a/JiawenHou_CorrGrid.xlsx
+++ b/JiawenHou_CorrGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Winnie/Dropbox/Study/COMP3004/A1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E9FD7-501A-0D40-BFA7-97E2B30A6796}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7896CB5E-72E8-DA4A-8D5E-7B86CED65DBC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="121">
   <si>
     <t>Your game starts</t>
   </si>
@@ -390,12 +390,6 @@
     <t>playerHitTwiceWin.txt</t>
   </si>
   <si>
-    <t>Manual</t>
-  </si>
-  <si>
-    <t>playersTest.java/testGetScoreAndAceHandler（）</t>
-  </si>
-  <si>
     <t>playerTest.java/testDealerHit()</t>
   </si>
   <si>
@@ -412,13 +406,19 @@
   </si>
   <si>
     <t>FileInputTests.java, 10 test cases in total</t>
+  </si>
+  <si>
+    <t>playersTest.java/testGetScoreAndAceHandler()</t>
+  </si>
+  <si>
+    <t>Please checkout README.md file for credential information(reference)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -455,12 +455,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Menlo"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -565,7 +559,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -576,7 +570,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -980,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="156" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1120,7 +1113,7 @@
         <v>0.5</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1135,7 +1128,7 @@
         <v>0.5</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1177,7 +1170,7 @@
       </c>
       <c r="C16" s="6"/>
       <c r="E16" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1361,7 +1354,7 @@
         <v>0.5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1478,7 +1471,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1753,8 +1746,8 @@
       <c r="D41">
         <v>3</v>
       </c>
-      <c r="E41" s="10" t="s">
-        <v>114</v>
+      <c r="E41" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -1777,7 +1770,7 @@
         <v>3</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -2006,7 +1999,7 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -2158,6 +2151,11 @@
       <c r="C75" s="7">
         <f>SUM(C6:C74)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>